<commit_message>
Początek testów manualnych - opisy w wordach i excelach
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Lp.</t>
   </si>
@@ -100,6 +100,24 @@
   </si>
   <si>
     <t>Wordy\Error KatPracownicy.docx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel administratora </t>
+  </si>
+  <si>
+    <t>Kontrola importu</t>
+  </si>
+  <si>
+    <t>Wordy\Panel admina importy.docx</t>
+  </si>
+  <si>
+    <t>Patrz Panel administratora</t>
+  </si>
+  <si>
+    <t>datapocz i datakoniec zły format ma być char 10</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -452,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -520,8 +538,14 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -610,6 +634,26 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1">
+        <v>43100</v>
       </c>
     </row>
   </sheetData>
@@ -620,9 +664,10 @@
     <hyperlink ref="F5" r:id="rId4"/>
     <hyperlink ref="I6" r:id="rId5"/>
     <hyperlink ref="F6" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Testy manualne początek do uzgodnienia
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Lp.</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Koszyk</t>
+  </si>
+  <si>
+    <t>Szczegół</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po kliknięciu na koszyk bez check-a </t>
+  </si>
+  <si>
+    <t>Wordy\Koszyk.docx</t>
   </si>
 </sst>
 </file>
@@ -470,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -656,6 +668,26 @@
         <v>43100</v>
       </c>
     </row>
+    <row r="9" spans="1:10" ht="28.5">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -665,9 +697,10 @@
     <hyperlink ref="I6" r:id="rId5"/>
     <hyperlink ref="F6" r:id="rId6"/>
     <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Opisy błędów w testy manualne - wysyłam na bieżąco
Hejt będzie trwał
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -120,16 +120,16 @@
     <t>H</t>
   </si>
   <si>
-    <t>Koszyk</t>
-  </si>
-  <si>
-    <t>Szczegół</t>
-  </si>
-  <si>
     <t xml:space="preserve">po kliknięciu na koszyk bez check-a </t>
   </si>
   <si>
     <t>Wordy\Koszyk.docx</t>
+  </si>
+  <si>
+    <t>Koszyk i teczki akt osobowych</t>
+  </si>
+  <si>
+    <t>Błędne komunikaty i brak nazwiska i imienia</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -668,24 +668,24 @@
         <v>43100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.5">
+    <row r="9" spans="1:10" ht="42.75">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="G9" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Błędy po testach manualnych
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Lp.</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Błędne komunikaty i brak nazwiska i imienia</t>
+  </si>
+  <si>
+    <t>Teczki akt osobowych</t>
+  </si>
+  <si>
+    <t>Wordy\Error Teczki akt osobowych.docx</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -688,6 +694,17 @@
         <v>34</v>
       </c>
     </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -698,9 +715,10 @@
     <hyperlink ref="F6" r:id="rId6"/>
     <hyperlink ref="D8" r:id="rId7"/>
     <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Uwagi merytoryczne - baaardzo ważne
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Lp.</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Wordy\Error Teczki akt osobowych.docx</t>
+  </si>
+  <si>
+    <t>Pliki - zapis do tabel</t>
+  </si>
+  <si>
+    <t>doprecyzowanie pól do zapisu</t>
+  </si>
+  <si>
+    <t>Wordy\Pliki zapisy do tabel.docx</t>
   </si>
 </sst>
 </file>
@@ -488,9 +497,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -705,6 +714,20 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="28.5">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -716,9 +739,10 @@
     <hyperlink ref="D8" r:id="rId7"/>
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Uwagi do modali i zapisów do tabel
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Lp.</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Wordy\Pliki zapisy do tabel.docx</t>
+  </si>
+  <si>
+    <t>Pliki - walidacja dat</t>
+  </si>
+  <si>
+    <t>modal git</t>
+  </si>
+  <si>
+    <t>Wordy\Walidacja dat Git.docx</t>
   </si>
 </sst>
 </file>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -728,6 +737,20 @@
         <v>42</v>
       </c>
     </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -740,9 +763,10 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Baza 9.00 z datami na character 10 i opisy błędów w pliku przygotowanie do prezentacji
</commit_message>
<xml_diff>
--- a/TESTY/Testy manualne.xlsx
+++ b/TESTY/Testy manualne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Lp.</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Wordy\Walidacja dat Git.docx</t>
+  </si>
+  <si>
+    <t>Przygotowanie do prezentacji</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Wordy\Przygotowanie do prezentacji.docx</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -517,7 +526,7 @@
     <col min="1" max="1" width="3.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
@@ -593,6 +602,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -611,7 +623,7 @@
     </row>
     <row r="5" spans="1:10" ht="28.5">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -637,7 +649,7 @@
     </row>
     <row r="6" spans="1:10" ht="28.5">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -663,7 +675,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -674,7 +686,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -694,7 +706,7 @@
     </row>
     <row r="9" spans="1:10" ht="42.75">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -714,7 +726,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
@@ -725,7 +737,7 @@
     </row>
     <row r="11" spans="1:10" ht="28.5">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -739,7 +751,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
@@ -749,6 +761,20 @@
       </c>
       <c r="D12" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -764,9 +790,10 @@
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
     <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>